<commit_message>
feat(Benchmark): added benchmark comparison script
</commit_message>
<xml_diff>
--- a/main/test/bonmin_tests.xlsx
+++ b/main/test/bonmin_tests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
   <si>
     <t xml:space="preserve">B-BB ALGORITHM</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">bonmin.algorithm B-Ecp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B-BB ALGORITHM + different efficiencies for pump1 (0.800) and pump2 (0.795) on ISGT</t>
   </si>
 </sst>
 </file>
@@ -92,11 +95,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -128,6 +132,16 @@
     </font>
     <font>
       <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -179,11 +193,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,7 +255,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -259,7 +273,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -299,14 +313,14 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0977156419194541"/>
-          <c:y val="0.216159052453469"/>
-          <c:w val="0.882222057405622"/>
-          <c:h val="0.693739424703892"/>
+          <c:x val="0.0861696581514858"/>
+          <c:y val="0.140883977900552"/>
+          <c:w val="0.881507410441647"/>
+          <c:h val="0.67210587177181"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -364,7 +378,16 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:val>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$E$8:$E$13</c:f>
               <c:numCache>
@@ -385,12 +408,9 @@
                 <c:pt idx="4">
                   <c:v>3950.45130014419</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>400.435910224915</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -449,7 +469,33 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:val>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$A$8:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>OSMSES</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OSMSES_2024Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ISGTbase</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ISGTcase1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ISGTcase2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ISGTcase3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$C$8:$C$13</c:f>
               <c:numCache>
@@ -475,7 +521,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -534,7 +580,33 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:val>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$A$8:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>OSMSES</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OSMSES_2024Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ISGTbase</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ISGTcase1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ISGTcase2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ISGTcase3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$C$23:$C$28</c:f>
               <c:numCache>
@@ -560,28 +632,173 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:hiLowLines>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="ffff00"/>
+            </a:solidFill>
+            <a:ln w="28800">
               <a:noFill/>
             </a:ln>
           </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="1"/>
-        <c:axId val="32880132"/>
-        <c:axId val="96278438"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="32880132"/>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffff00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$A$8:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>OSMSES</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OSMSES_2024Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ISGTbase</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ISGTcase1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ISGTcase2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ISGTcase3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$38:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.05224347114563</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.05224347114563</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160.66055059433</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>182.706394910812</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>698.927576780319</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1803.48035597801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="23163295"/>
+        <c:axId val="64628586"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="23163295"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-1200000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="800" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64628586"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64628586"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -603,55 +820,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96278438"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="96278438"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="32880132"/>
+        <c:crossAx val="23163295"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -663,7 +834,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="span"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -676,7 +847,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -716,14 +887,15 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0601366380680012"/>
-          <c:y val="0.14901269393512"/>
-          <c:w val="0.920082618366699"/>
-          <c:h val="0.761212976022567"/>
+          <c:x val="0.0601357904946654"/>
+          <c:y val="0.149026361107431"/>
+          <c:w val="0.920017906438857"/>
+          <c:h val="0.76116041859849"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -743,19 +915,165 @@
             <a:solidFill>
               <a:srgbClr val="2a6099"/>
             </a:solidFill>
-            <a:ln w="28800">
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="2a6099"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$8:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-9.71570586443242E-009</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9.71570586443242E-009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.14779361909799E-006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00119929033824642</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.0058949810547353</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0139795840935166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$22:$H$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Goal_dif</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff8000"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$23:$H$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-9.71109546844714E-009</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9.71109546844714E-009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00170454403140793</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0899406706437904</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.183069249635404</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.0093289179789186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Goal_dif</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:txPr>
               <a:bodyPr wrap="none"/>
@@ -783,7 +1101,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$8:$H$13</c:f>
+              <c:f>Sheet1!$H$38:$H$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -794,126 +1112,34 @@
                   <c:v>-9.71570586443242E-009</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.14779361909799E-006</c:v>
+                  <c:v>0.00216289046360693</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00119929033824642</c:v>
+                  <c:v>0.0162214413380406</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.0058949810547353</c:v>
+                  <c:v>-0.00296044367759655</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0139795840935166</c:v>
+                  <c:v>0.00549427533935322</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$22:$H$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Goal_dif</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff8000"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff8000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$23:$H$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>-9.71109546844714E-009</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-9.71109546844714E-009</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.00170454403140793</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0899406706437904</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.183069249635404</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.0093289179789186</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="1"/>
-        <c:axId val="95900557"/>
-        <c:axId val="37264088"/>
-      </c:lineChart>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="53202556"/>
+        <c:axId val="60041791"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="95900557"/>
+        <c:axId val="53202556"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -935,7 +1161,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37264088"/>
+        <c:crossAx val="60041791"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -943,7 +1169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37264088"/>
+        <c:axId val="60041791"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -958,7 +1184,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -980,9 +1206,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95900557"/>
+        <c:crossAx val="53202556"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1011,16 +1237,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>808920</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>795600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:colOff>765720</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1028,8 +1254,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7746480" y="162720"/>
-        <a:ext cx="4853880" cy="2553120"/>
+        <a:off x="7736760" y="248760"/>
+        <a:ext cx="4833720" cy="2801880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1041,16 +1267,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>41400</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>725400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>802440</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>106920</xdr:rowOff>
+      <xdr:colOff>673200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1058,8 +1284,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7782120" y="2916360"/>
-        <a:ext cx="4825080" cy="2717640"/>
+        <a:off x="7653240" y="3165480"/>
+        <a:ext cx="4824720" cy="2717280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1077,10 +1303,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1289,9 +1515,6 @@
       <c r="D13" s="1" t="n">
         <v>-30.2289351273265</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <v>400.435910224915</v>
-      </c>
       <c r="F13" s="1" t="n">
         <v>2456</v>
       </c>
@@ -1516,6 +1739,280 @@
         <f aca="false">(B28-D28)/ABS(D28)</f>
         <v>-0.0093289179789186</v>
       </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>-1918.06020556249</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>1.05224347114563</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>-1918.06018692718</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>16.7859210968018</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <f aca="false">(B38-D38)/ABS(D38)</f>
+        <v>-9.71570586443242E-009</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>-1918.06020556249</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>1.05224347114563</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>-1918.06018692718</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>5.869357049</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="G39" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <f aca="false">(B39-D39)/ABS(D39)</f>
+        <v>-9.71570586443242E-009</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>25.0172260338746</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>160.66055059433</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>24.9632332946408</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>508.147188186646</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>2070</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>2166</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <f aca="false">(B40-D40)/ABS(D40)</f>
+        <v>0.00216289046360693</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>13.1141526587402</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>182.706394910812</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>12.9048179120026</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>679.132902383804</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>2456</v>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>2456</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <f aca="false">(B41-D41)/ABS(D41)</f>
+        <v>0.0162214413380406</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>-29.5977478720774</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>698.927576780319</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>-29.5103840422162</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>3950.45130014419</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>2070</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>2070</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <f aca="false">(B42-D42)/ABS(D42)</f>
+        <v>-0.00296044367759655</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>-30.0628490345215</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>1803.48035597801</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>-30.2289351273265</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>400.435910224915</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>2456</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>2550</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <f aca="false">(B43-D43)/ABS(D43)</f>
+        <v>0.00549427533935322</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="0"/>
+      <c r="D48" s="0"/>
+      <c r="E48" s="0"/>
+      <c r="F48" s="0"/>
+      <c r="G48" s="0"/>
+      <c r="H48" s="0"/>
+      <c r="I48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="0"/>
+      <c r="D49" s="0"/>
+      <c r="E49" s="0"/>
+      <c r="F49" s="0"/>
+      <c r="G49" s="0"/>
+      <c r="H49" s="0"/>
+      <c r="I49" s="0"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+      <c r="E50" s="0"/>
+      <c r="F50" s="0"/>
+      <c r="G50" s="0"/>
+      <c r="H50" s="0"/>
+      <c r="I50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
+      <c r="E51" s="0"/>
+      <c r="F51" s="0"/>
+      <c r="G51" s="0"/>
+      <c r="H51" s="0"/>
+      <c r="I51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="0"/>
+      <c r="D52" s="0"/>
+      <c r="E52" s="0"/>
+      <c r="F52" s="0"/>
+      <c r="G52" s="0"/>
+      <c r="H52" s="0"/>
+      <c r="I52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="0"/>
+      <c r="D53" s="0"/>
+      <c r="E53" s="0"/>
+      <c r="F53" s="0"/>
+      <c r="G53" s="0"/>
+      <c r="H53" s="0"/>
+      <c r="I53" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>